<commit_message>
Add more acquisition instrument models for LC-MS.
Closes #74
</commit_message>
<xml_diff>
--- a/lcms/latest/lcms.xlsx
+++ b/lcms/latest/lcms.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="429">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -577,6 +577,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
+    <t>MS Lipidomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
+  </si>
+  <si>
     <t>analyte_class</t>
   </si>
   <si>
@@ -724,6 +730,12 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Vizgen</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026274</t>
+  </si>
+  <si>
     <t>Standard BioTools (Fluidigm)</t>
   </si>
   <si>
@@ -877,6 +889,12 @@
     <t>https://identifiers.org/RRID:SCR_021658</t>
   </si>
   <si>
+    <t>timsTOF Ultra 2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026541</t>
+  </si>
+  <si>
     <t>Lightsheet 7</t>
   </si>
   <si>
@@ -895,12 +913,24 @@
     <t>https://identifiers.org/RRID:SCR_024847</t>
   </si>
   <si>
+    <t>timsTOF Pro</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026544</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
   </si>
   <si>
+    <t>timsTOF Pro 2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026545</t>
+  </si>
+  <si>
     <t>Q Exactive UHMR</t>
   </si>
   <si>
@@ -913,6 +943,12 @@
     <t>https://identifiers.org/RRID:SCR_020565</t>
   </si>
   <si>
+    <t>timsTOF SCP</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026542</t>
+  </si>
+  <si>
     <t>Zyla 4.2 sCMOS</t>
   </si>
   <si>
@@ -931,6 +967,12 @@
     <t>https://identifiers.org/RRID:SCR_020517</t>
   </si>
   <si>
+    <t>timsTOF Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026540</t>
+  </si>
+  <si>
     <t>BZ-X800</t>
   </si>
   <si>
@@ -1003,6 +1045,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>timsTOF HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026543</t>
+  </si>
+  <si>
     <t>PhenoImager Fusion</t>
   </si>
   <si>
@@ -1081,6 +1129,12 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>MERSCOPE</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000404</t>
+  </si>
+  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -1123,6 +1177,12 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
+    <t>MERSCOPE Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026273</t>
+  </si>
+  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1555,7 +1615,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-01-08T12:46:05-08:00</t>
+    <t>2025-03-08T07:35:05-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1743,130 +1803,130 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>393</v>
+        <v>413</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>400</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2">
@@ -1874,13 +1934,13 @@
         <v>64</v>
       </c>
       <c r="AT2" t="s" s="47">
-        <v>401</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="32">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$38</formula1>
+      <formula1>'dataset_type'!$A$1:$A$39</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1889,10 +1949,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$60</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2003,26 +2063,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>307</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2040,26 +2100,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>314</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -2077,50 +2137,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>323</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>325</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>327</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>329</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>331</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>333</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2138,34 +2198,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>336</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>338</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>340</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>342</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2183,58 +2243,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>348</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>350</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2252,50 +2312,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>350</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2313,26 +2373,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2350,10 +2410,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>368</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2371,26 +2431,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>364</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2408,18 +2468,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>374</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>376</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2737,6 +2797,14 @@
       </c>
       <c r="B38" t="s" s="0">
         <v>79</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2754,10 +2822,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2775,10 +2843,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>383</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2">
@@ -2786,39 +2854,39 @@
         <v>66</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>384</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>386</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>388</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>390</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>392</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -2836,18 +2904,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>396</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>397</v>
+        <v>417</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>398</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2871,16 +2939,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>403</v>
+        <v>423</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>407</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2">
@@ -2888,13 +2956,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>406</v>
+        <v>426</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>408</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -2912,130 +2980,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3053,12 +3121,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3068,7 +3136,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3076,186 +3144,194 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3265,7 +3341,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3273,418 +3349,482 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>267</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>276</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>282</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3702,42 +3842,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3755,26 +3895,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3792,42 +3932,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>286</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>288</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>292</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>294</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6">
@@ -3835,7 +3975,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7">
@@ -3843,31 +3983,31 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>296</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>298</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>302</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a new MS ionization technique "nESI"
Closes #121
</commit_message>
<xml_diff>
--- a/lcms/latest/lcms.xlsx
+++ b/lcms/latest/lcms.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="494">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -361,34 +361,166 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>CosMx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -397,36 +529,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -457,16 +559,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -475,24 +571,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -523,18 +607,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -547,12 +619,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -565,34 +631,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -730,6 +778,18 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -844,12 +904,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -883,6 +955,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -991,6 +1069,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1069,6 +1153,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1105,6 +1195,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1195,6 +1291,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1219,6 +1318,18 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1231,6 +1342,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1255,6 +1372,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1372,6 +1495,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000279</t>
   </si>
   <si>
+    <t>nESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000456</t>
+  </si>
+  <si>
     <t>ms_scan_mode</t>
   </si>
   <si>
@@ -1681,7 +1810,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:16:33-07:00</t>
+    <t>2025-09-25T16:07:11-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1869,144 +1998,144 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>351</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>352</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>345</v>
+        <v>388</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>352</v>
+        <v>395</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>385</v>
+        <v>428</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>393</v>
+        <v>436</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>394</v>
+        <v>437</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>397</v>
+        <v>440</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>398</v>
+        <v>441</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>399</v>
+        <v>442</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>400</v>
+        <v>443</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>407</v>
+        <v>450</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>408</v>
+        <v>451</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>411</v>
+        <v>454</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>412</v>
+        <v>455</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>413</v>
+        <v>456</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>414</v>
+        <v>457</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>419</v>
+        <v>462</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>420</v>
+        <v>463</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>421</v>
+        <v>464</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>422</v>
+        <v>465</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>423</v>
+        <v>466</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>435</v>
+        <v>478</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>436</v>
+        <v>479</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>441</v>
+        <v>484</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>442</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="AT2" t="s" s="47">
-        <v>443</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="32">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2015,10 +2144,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2035,7 +2164,7 @@
       <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'ms_ionization_technique'!$A$1:$A$10</formula1>
+      <formula1>'ms_ionization_technique'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'ms_scan_mode'!$A$1:$A$3</formula1>
@@ -2129,26 +2258,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>347</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>349</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>351</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2166,26 +2295,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>400</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -2203,50 +2332,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>365</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>367</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>368</v>
+        <v>411</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>369</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>371</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>373</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>375</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2264,34 +2393,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>378</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>379</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>380</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>381</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>382</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>384</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2309,58 +2438,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>388</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>390</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>392</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2378,50 +2507,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>396</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>388</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>392</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2439,26 +2568,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>401</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>402</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>403</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>404</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>405</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>406</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -2476,10 +2605,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>409</v>
+        <v>452</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>410</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -2497,26 +2626,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>401</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>402</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>403</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>404</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>405</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>406</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -2534,18 +2663,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>415</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>416</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>417</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>418</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -2555,7 +2684,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2887,6 +3016,70 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2904,10 +3097,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>361</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2925,50 +3118,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>424</v>
+        <v>467</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>425</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>426</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>427</v>
+        <v>470</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>428</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>429</v>
+        <v>472</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>430</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>431</v>
+        <v>474</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>432</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>433</v>
+        <v>476</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>434</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -2986,18 +3179,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>438</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>439</v>
+        <v>482</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>440</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -3021,30 +3214,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>444</v>
+        <v>487</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>445</v>
+        <v>488</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>447</v>
+        <v>490</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>449</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>446</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>448</v>
+        <v>491</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>450</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -3062,130 +3255,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3203,12 +3396,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3218,7 +3411,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3226,210 +3419,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +3664,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3447,546 +3672,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>169</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>333</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4004,42 +4301,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4057,26 +4354,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4086,7 +4383,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4094,82 +4391,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>328</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>329</v>
+        <v>370</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>330</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>331</v>
+        <v>372</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>332</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>333</v>
+        <v>374</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>334</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>335</v>
+        <v>376</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>336</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>337</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>338</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>339</v>
+        <v>380</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>340</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>342</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>343</v>
+        <v>384</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>344</v>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update LCMS metadata templates to use updated field descriptions
</commit_message>
<xml_diff>
--- a/lcms/latest/lcms.xlsx
+++ b/lcms/latest/lcms.xlsx
@@ -42,128 +42,137 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) The ionization approach (i.e., sample probing method) for performing
-imaging mass spectrometry.</t>
+        <t>(Required) The ionization technique used in imaging mass spectrometry, which
+refers to the method employed to probe the sample. Example: MALDI</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) MS (mass spectrometry) scan mode refers to the number of steps in the
-separation of fragments.</t>
+        <t>(Required) The mode of mass spectrometry (MS) scanning, which refers to the
+number of steps involved in the separation of fragments during the analysis.
+Example: MS1</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The polarity of the mass analysis (positive or negative ion modes).</t>
+        <t>(Required) The polarity mode used in mass analysis, indicating whether positive
+or negative ion modes are employed. Example: Positive ion mode</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>The low value of the scanned mass-to-charge range, for MS1. (unitless)</t>
+        <t>The low value of the scanned mass-to-charge range for MS1. This value is
+unitless. Example: 100</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
@@ -173,65 +182,75 @@
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>The mass resolving power m/∆m, where ∆m is defined as the full width at
-half-maximum (FWHM) for a given peak with a specified mass-to-charge (m/z).
-(unitless)</t>
+        <t>The mass resolving power, denoted as m/∆m, where ∆m is defined as the full width
+at half-maximum (FWHM) for a given peak with a specified mass-to-charge ratio
+(m/z). This measurement is unitless. Example: 60000</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>The peak (m/z) used to calculate the resolving power.</t>
+        <t>The peak mass-to-charge ratio (m/z) used to calculate the resolving power.
+Example: 400.2</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>Specifies which technology was used for ion mobility spectrometry. Technologies
-for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS),
-Trapped Ion Mobility Spectrometry (TIMS), High Field Asymmetric waveform ion
-Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS),
-Structures for Lossless Ion Manipulations (SLIM), and cyclic Ion Mobility
-Spectrometry (cIMS).</t>
+        <t>The specific technology employed for ion mobility spectrometry. Available
+technologies include Traveling Wave Ion Mobility Spectrometry (TWIMS), Trapped
+Ion Mobility Spectrometry (TIMS), High Field Asymmetric Waveform Ion Mobility
+Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS), Structures
+for Lossless Ion Manipulations (SLIM), and cyclic Ion Mobility Spectrometry
+(cIMS). Example: TIMS</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent
-acquisition), DIA (Data-independent acquisition), SRM (multiple reaction
-monitoring), or PRM (parallel reaction monitoring).</t>
+        <t>The mode of data collection used in tandem MS assays, which can include options
+such as Data-dependent acquisition (DDA), Data-independent acquisition (DIA),
+multiple reaction monitoring (SRM), or parallel reaction monitoring (PRM).
+Example: PRM</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>If the samples were labeled (e.g. TMT), provide the name/ID of the label on this
-sample. Leave blank if not applicable.</t>
+        <t>The name or identifier of the chemical label used on this sample if labeling was
+applied. This is typically required for multiplexed experiments using techniques
+like Tandem Mass Tag (TMT). If sample was not labeled, this field may be left
+blank. Example: TMT126</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>The manufacturer of the instrument used for liquid chromatography.</t>
+        <t>The company that manufactures the instrument used for liquid chromatography. If
+the instrument was custom-built or developed internally, enter "In-House".
+Example: Bruker</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>The model number/name of the instrument used for liquid chromatography.</t>
+        <t>The model number or name of the instrument used for liquid chromatography.
+Example: Bruker Elute LC-MS</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>The manufacturer of the liquid chromatography column unless self-packed, pulled
-tip capillary is used.</t>
+        <t>The manufacturer of the liquid chromatography column used, unless a self-packed
+or pulled tip capillary is employed. If the column was custom-made or developed
+internally, enter "In-House". Example: Bruker</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>The model number/name of the liquid chromatography column. If it is a custom
-self-packed, pulled tip capillary is used enter “Pulled tip capilary”.</t>
+        <t>The model number or name of the liquid chromatography column used. If a custom
+self-packed, pulled tip capillary is utilized, enter "Pulled tip capillary".
+Example: Thermo Scientific Vanquish UHPLC</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>Details of the resin used for liquid chromatography, including vendor, particle
-size, pore size.</t>
+        <t>The details of the resin used in liquid chromatography, including information
+about the vendor, particle size, and pore size. Example: Thermo Fisher
+Scientific, Acclaim PepMap 100 C18, 3 µm, 100 Å</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
@@ -246,7 +265,8 @@
     </comment>
     <comment ref="AF1" authorId="1">
       <text>
-        <t>Liquid chromatography temperature.</t>
+        <t>The temperature at which the liquid chromatography (LC) process is conducted.
+Example: 40</t>
       </text>
     </comment>
     <comment ref="AG1" authorId="1">
@@ -261,7 +281,8 @@
     </comment>
     <comment ref="AI1" authorId="1">
       <text>
-        <t/>
+        <t>The unit of measurment for the LC inner diameter value. If the diameter is not
+specified, this field may be left blank. Example: um</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="1">
@@ -276,7 +297,7 @@
     </comment>
     <comment ref="AL1" authorId="1">
       <text>
-        <t>Liquid chromatography gradient.</t>
+        <t>The liquid chromatography (LC) gradient used in the assay. Example: 120</t>
       </text>
     </comment>
     <comment ref="AM1" authorId="1">
@@ -301,19 +322,19 @@
     </comment>
     <comment ref="AQ1" authorId="1">
       <text>
-        <t>Specifies the cell-type or functional tissue unit (FTU) that is targeted in the
-spatial profiling experiment. Leave blank if data are generated in imaging mode
-without a specific target structure.</t>
+        <t>The cell type or functional tissue unit (FTU) that is the focus of the spatial
+profiling experiment. If the data are generated in imaging mode without
+targeting a specific structure, this field may be left blank. Example: Proximal
+tubule epithelial cell</t>
       </text>
     </comment>
     <comment ref="AR1" authorId="1">
       <text>
-        <t>Specifies whether or not the analysis was performed in a spatially targeted
-manner. Spatial profiling experiments target specific tissue foci but do not
-necessarily generate images. Spatial imaging expriments collect data from a
-regular array (pixels) that can be visualized as heat maps of ion intensity at
-each location (molecular images). Leave blank if data are derived from bulk
-analysis.</t>
+        <t>The type of spatial targeting used in the analysis. Spatial profiling focuses on
+selected tissue regions without necessarily producing images, while spatial
+imaging captures data across a regular grid of pixels, enabling visualization as
+ion intensity heat maps—also referred to as molecular images. Leave this field
+blank if the data originate from bulk (non-spatial) analysis. Example: Imaging</t>
       </text>
     </comment>
     <comment ref="AS1" authorId="1">
@@ -325,8 +346,8 @@
     </comment>
     <comment ref="AT1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -335,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="496">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -361,6 +382,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
     <t>Visium (no probes)</t>
   </si>
   <si>
@@ -397,24 +424,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>CosMx</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -1810,7 +1837,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-09-25T16:07:11-07:00</t>
+    <t>2025-10-20T14:51:07-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1998,144 +2025,144 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT2" t="s" s="47">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="32">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$49</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2258,26 +2285,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -2295,26 +2322,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -2332,50 +2359,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -2393,34 +2420,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -2438,58 +2465,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -2507,50 +2534,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -2568,26 +2595,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -2605,10 +2632,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -2626,26 +2653,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -2663,18 +2690,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2711,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3080,6 +3107,14 @@
       </c>
       <c r="B49" t="s" s="0">
         <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3097,10 +3132,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3118,50 +3153,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -3179,18 +3214,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3214,30 +3249,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -3255,130 +3290,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3396,12 +3431,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3419,242 +3454,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3672,618 +3707,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4301,42 +4336,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4354,26 +4389,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4391,90 +4426,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>